<commit_message>
fix problem Import Data di template AdminLTE
</commit_message>
<xml_diff>
--- a/public/DataPegawai/Daftar Karyawan Wakaf Salman Impor.xlsx
+++ b/public/DataPegawai/Daftar Karyawan Wakaf Salman Impor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0A3A81-C105-4E28-8E5E-A7EA8D22B808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB4BAB3-3D3A-4D39-8B0E-C6ACDF35A36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -57,16 +57,16 @@
     <t>2022-01-25T04:44:23.000000Z</t>
   </si>
   <si>
-    <t>Radian Pradhana</t>
-  </si>
-  <si>
-    <t>Rian</t>
-  </si>
-  <si>
-    <t>Rian Pradhana</t>
-  </si>
-  <si>
-    <t>Ryan</t>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>

</xml_diff>